<commit_message>
add type stat pdfs
</commit_message>
<xml_diff>
--- a/excels/manual.xlsx
+++ b/excels/manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\36706\Workspaces\viatra-workspace\Structural-Analysis-of-Partial-Models-using-Graph-Metrics\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B392481-01DD-4523-B176-E892DD74A3FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C70289-1A5A-4EE8-A3AF-F52D692F3CC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9D0E90E0-6524-4963-A7D1-13008B857362}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="10" xr2:uid="{9D0E90E0-6524-4963-A7D1-13008B857362}"/>
   </bookViews>
   <sheets>
     <sheet name="step-1" sheetId="2" r:id="rId1"/>
@@ -21,10 +21,11 @@
     <sheet name="step-6" sheetId="7" r:id="rId6"/>
     <sheet name="step-7" sheetId="8" r:id="rId7"/>
     <sheet name="step-8" sheetId="9" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId9"/>
+    <sheet name="osszesitett" sheetId="10" r:id="rId9"/>
+    <sheet name="osszesitett-2" sheetId="12" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="5">
   <si>
     <t>Statechart</t>
   </si>
@@ -100,11 +101,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEA526F"/>
+      <color rgb="FFFADF63"/>
+      <color rgb="FFC4A69D"/>
       <color rgb="FFE7E6F7"/>
-      <color rgb="FFC4A69D"/>
-      <color rgb="FFEA526F"/>
       <color rgb="FF20A39E"/>
-      <color rgb="FFFADF63"/>
       <color rgb="FFE70000"/>
     </mruColors>
   </colors>
@@ -432,6 +433,539 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Statechart</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E7E6F7"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$3:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8DCF-4F7C-A295-D8CCB880C406}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Region</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C4A69D"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$3:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8DCF-4F7C-A295-D8CCB880C406}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Entry</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FADF63"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8DCF-4F7C-A295-D8CCB880C406}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>State</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="EA526F"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8DCF-4F7C-A295-D8CCB880C406}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Transition</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="20A39E"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$3:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8DCF-4F7C-A295-D8CCB880C406}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1649695280"/>
+        <c:axId val="1596985856"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1649695280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1596985856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1596985856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1649695280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2596,7 +3130,572 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Statechart</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E7E6F7"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$3:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E2EA-4EAD-B79D-04FF375657B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Region</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C4A69D"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$3:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E2EA-4EAD-B79D-04FF375657B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Entry</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FADF63"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E2EA-4EAD-B79D-04FF375657B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>State</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="EA526F"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E2EA-4EAD-B79D-04FF375657B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Transition</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="20A39E"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$3:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E2EA-4EAD-B79D-04FF375657B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1649695280"/>
+        <c:axId val="1596985856"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="1649695280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1596985856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1596985856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1649695280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2916,6 +4015,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3419,8 +4558,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3624,22 +4763,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -3689,9 +4829,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:floor>
@@ -3744,8 +4889,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3809,6 +4954,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -3877,19 +5033,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3922,7 +5079,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4425,7 +5582,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4928,7 +6085,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5431,7 +6588,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5934,7 +7091,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6437,7 +7594,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6940,14 +8097,1051 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BA597C31-EDBF-4E80-B62E-9443D0B7E98D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C3609C8E-A5C4-4258-9C31-4DD419AD3EDE}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -6958,7 +9152,8 @@
     <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -6969,7 +9164,8 @@
     <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -6980,7 +9176,8 @@
     <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -6991,7 +9188,8 @@
     <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -7002,7 +9200,8 @@
     <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -7013,7 +9212,8 @@
     <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -7024,7 +9224,20 @@
     <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{86566CD2-A123-4618-8E90-836FB0D624FF}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -7032,7 +9245,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298112" cy="6070315"/>
+    <xdr:ext cx="9291205" cy="6070023"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7061,11 +9274,44 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9291205" cy="6070023"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC604D9A-49E4-467D-8C8B-3EE272767310}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298112" cy="6070315"/>
+    <xdr:ext cx="9291205" cy="6070023"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7098,7 +9344,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298112" cy="6070315"/>
+    <xdr:ext cx="9291205" cy="6070023"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7131,7 +9377,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298112" cy="6070315"/>
+    <xdr:ext cx="9291205" cy="6070023"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7164,7 +9410,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298112" cy="6070315"/>
+    <xdr:ext cx="9291205" cy="6070023"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7197,7 +9443,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298112" cy="6070315"/>
+    <xdr:ext cx="9291205" cy="6070023"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7230,7 +9476,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298112" cy="6070315"/>
+    <xdr:ext cx="9291205" cy="6070023"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7263,13 +9509,46 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298112" cy="6070315"/>
+    <xdr:ext cx="9291205" cy="6070023"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6F3D83D-4AD4-469D-8770-E9E632FF399D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9291205" cy="6070023"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9828D087-E9F2-4738-8616-5809FC782C9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7589,10 +9868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50AC7CCA-3ED0-417E-BB5C-3093596C6378}">
-  <dimension ref="B2:F17"/>
+  <dimension ref="B2:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7600,7 +9879,7 @@
     <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -7616,8 +9895,23 @@
       <c r="F2" t="s">
         <v>4</v>
       </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -7633,8 +9927,26 @@
       <c r="F3">
         <v>3</v>
       </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -7650,8 +9962,26 @@
       <c r="F4" t="s">
         <v>4</v>
       </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
@@ -7667,8 +9997,26 @@
       <c r="F5">
         <v>3</v>
       </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -7684,8 +10032,26 @@
       <c r="F6" t="s">
         <v>4</v>
       </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1</v>
       </c>
@@ -7701,8 +10067,26 @@
       <c r="F7">
         <v>2</v>
       </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -7718,8 +10102,26 @@
       <c r="F8" t="s">
         <v>4</v>
       </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1</v>
       </c>
@@ -7735,8 +10137,26 @@
       <c r="F9">
         <v>2</v>
       </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>0</v>
       </c>
@@ -7752,8 +10172,26 @@
       <c r="F10" t="s">
         <v>4</v>
       </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1</v>
       </c>
@@ -7770,7 +10208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -7787,7 +10225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>1</v>
       </c>
@@ -7804,7 +10242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -7821,7 +10259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>1</v>
       </c>
@@ -7838,7 +10276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>0</v>
       </c>

</xml_diff>